<commit_message>
Added default value column
</commit_message>
<xml_diff>
--- a/Resources/fixtures/minimal_FR/init.xlsx
+++ b/Resources/fixtures/minimal_FR/init.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4005" tabRatio="226"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4005" tabRatio="226" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="10" r:id="rId1"/>
@@ -23,8 +23,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">attribute_groups!$A$4:$C$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AX$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$AZ$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">attributes!$B$6:$AY$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'family main'!$C$6:$BA$9</definedName>
     <definedName name="boolean_choices">choices!$A$1:$A$2</definedName>
     <definedName name="date_choices">choices!$C$1:$C$3</definedName>
     <definedName name="validation_choices">choices!$B$1:$B$3</definedName>
@@ -40,73 +40,6 @@
   </authors>
   <commentList>
     <comment ref="I5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Spécifier le nom des locales, séparées par ","
-Par exemple : "en_US, fr_FR"
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Inscrire les extensions permises, séparées par une ","
-Par exemple : 
-jpg, jpeg, png</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Spécifie le nombre de caractères à taper pour avoir une liste d'options, pour les attributs de type select.
-Cette option doit être utilisée si de nombreuses options sont proposées</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>SMILE</author>
-  </authors>
-  <commentList>
-    <comment ref="AD4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Insérer 1 si l'attribut est requis pour cette famille et ce canal</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -137,6 +70,73 @@
       </text>
     </comment>
     <comment ref="AC5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Spécifie le nombre de caractères à taper pour avoir une liste d'options, pour les attributs de type select.
+Cette option doit être utilisée si de nombreuses options sont proposées</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SMILE</author>
+  </authors>
+  <commentList>
+    <comment ref="AE4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Insérer 1 si l'attribut est requis pour cette famille et ce canal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Spécifier le nom des locales, séparées par ","
+Par exemple : "en_US, fr_FR"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Inscrire les extensions permises, séparées par une ","
+Par exemple : 
+jpg, jpeg, png</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="275">
   <si>
     <t>en_US</t>
   </si>
@@ -1137,6 +1137,15 @@
       </rPr>
       <t>Le titre de l'onglet devra commencer par "attributes"</t>
     </r>
+  </si>
+  <si>
+    <t>²</t>
+  </si>
+  <si>
+    <t>default_value</t>
+  </si>
+  <si>
+    <t>Valeur par défaut</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1341,6 +1350,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1985,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3199,10 +3209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY8"/>
+  <dimension ref="A1:AZ19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3218,48 +3228,48 @@
     <col min="9" max="9" width="25.140625" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.5703125" style="16" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="16" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5703125" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" customWidth="1"/>
-    <col min="25" max="25" width="26.42578125" customWidth="1"/>
-    <col min="26" max="26" width="23.140625" customWidth="1"/>
-    <col min="27" max="27" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="34.5703125" customWidth="1"/>
-    <col min="48" max="48" width="9.140625" style="2"/>
-    <col min="49" max="49" width="9.140625" style="3"/>
-    <col min="50" max="51" width="9.140625" style="2"/>
+    <col min="12" max="13" width="29.7109375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" customWidth="1"/>
+    <col min="26" max="26" width="26.42578125" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="34.5703125" customWidth="1"/>
+    <col min="49" max="49" width="9.140625" style="2"/>
+    <col min="50" max="50" width="9.140625" style="3"/>
+    <col min="51" max="52" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>267</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="AV1"/>
       <c r="AW1"/>
       <c r="AX1"/>
       <c r="AY1"/>
-    </row>
-    <row r="2" spans="1:51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AZ1"/>
+    </row>
+    <row r="2" spans="1:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="AV2"/>
       <c r="AW2"/>
       <c r="AX2"/>
       <c r="AY2"/>
-    </row>
-    <row r="4" spans="1:51" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AZ2"/>
+    </row>
+    <row r="4" spans="1:52" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -3292,8 +3302,9 @@
       <c r="Z4" s="30"/>
       <c r="AA4" s="30"/>
       <c r="AB4" s="30"/>
-    </row>
-    <row r="5" spans="1:51" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC4" s="30"/>
+    </row>
+    <row r="5" spans="1:52" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>205</v>
       </c>
@@ -3331,55 +3342,58 @@
         <v>218</v>
       </c>
       <c r="M5" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="N5" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="O5" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="P5" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="R5" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="S5" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="S5" s="25" t="s">
+      <c r="T5" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="T5" s="25" t="s">
+      <c r="U5" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="V5" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="W5" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="W5" s="25" t="s">
+      <c r="X5" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="X5" s="25" t="s">
+      <c r="Y5" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="Y5" s="25" t="s">
+      <c r="Z5" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="AA5" s="25" t="s">
+      <c r="AB5" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="AB5" s="25" t="s">
+      <c r="AC5" s="25" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:51" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -3416,60 +3430,63 @@
       <c r="L6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="W6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="X6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Z6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AA6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AB6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AV6"/>
       <c r="AW6"/>
       <c r="AX6"/>
       <c r="AY6"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ6"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
@@ -3504,8 +3521,8 @@
       <c r="L7" s="18">
         <v>1</v>
       </c>
-      <c r="M7" s="11"/>
-      <c r="O7" s="11"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
@@ -3538,14 +3555,15 @@
       <c r="AS7" s="11"/>
       <c r="AT7" s="11"/>
       <c r="AU7" s="11"/>
-      <c r="AV7" s="2" t="s">
+      <c r="AV7" s="11"/>
+      <c r="AW7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AX7" s="2">
+      <c r="AY7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3579,36 +3597,42 @@
       <c r="L8" s="16">
         <v>1</v>
       </c>
+      <c r="W8" s="33"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="16" t="s">
+        <v>272</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C4:AB4"/>
+    <mergeCell ref="C4:AC4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA7:AA1048576"/>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="Q7:R1048576">
+  <dataValidations disablePrompts="1" count="17">
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB7:AB1048576"/>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="R7:S1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="Z7:Z1048576 AB7:AB1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AA7:AA1048576 AC7:AC1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:U1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N7:N1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O7:O1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7:M1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:L1048576 P7:P1048576 S7:T1048576 F7:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:H1048576 Q7:Q1048576 T7:U1048576 J7:L1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3616,31 +3640,31 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7 AP7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7 AQ7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
-      <formula1>$Q$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7">
+      <formula1>$R$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7:AM7 AR7:AT7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7:AN7 AS7:AU7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3650,7 +3674,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>attribute_types!$B$3:$B$14</xm:f>
@@ -3661,13 +3685,13 @@
           <x14:formula1>
             <xm:f>metric_units!$B$3:$B$89</xm:f>
           </x14:formula1>
-          <xm:sqref>Y7:Y1048576</xm:sqref>
+          <xm:sqref>Z7:Z1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>metric_types!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>X7:X1048576</xm:sqref>
+          <xm:sqref>Y7:Y1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
@@ -3683,10 +3707,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA8"/>
+  <dimension ref="A1:BB8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3702,48 +3726,48 @@
     <col min="10" max="10" width="25.140625" customWidth="1"/>
     <col min="11" max="11" width="23.5703125" style="16"/>
     <col min="12" max="12" width="34.5703125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="16" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125"/>
-    <col min="15" max="15" width="19.28515625"/>
-    <col min="16" max="16" width="25.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625"/>
-    <col min="18" max="18" width="16.5703125"/>
-    <col min="19" max="19" width="19"/>
-    <col min="20" max="20" width="21.42578125" customWidth="1"/>
-    <col min="21" max="21" width="18.7109375"/>
-    <col min="22" max="23" width="13.42578125"/>
-    <col min="24" max="24" width="19.85546875"/>
-    <col min="25" max="25" width="20.42578125" customWidth="1"/>
-    <col min="26" max="26" width="26.42578125" customWidth="1"/>
-    <col min="27" max="27" width="21"/>
-    <col min="28" max="28" width="22"/>
-    <col min="29" max="29" width="34.5703125" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" style="16"/>
-    <col min="31" max="39" width="13.42578125"/>
-    <col min="40" max="40" width="16.85546875"/>
-    <col min="41" max="41" width="19.140625"/>
-    <col min="42" max="42" width="16.28515625"/>
-    <col min="43" max="45" width="13.42578125"/>
-    <col min="46" max="46" width="19.140625"/>
-    <col min="47" max="49" width="18.140625"/>
-    <col min="50" max="50" width="0" style="2" hidden="1"/>
-    <col min="51" max="51" width="0" style="3" hidden="1"/>
-    <col min="52" max="52" width="0" style="2" hidden="1"/>
-    <col min="53" max="53" width="17.140625" style="2"/>
-    <col min="54" max="1024" width="17.140625"/>
+    <col min="13" max="14" width="29.7109375" style="16" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125"/>
+    <col min="16" max="16" width="19.28515625"/>
+    <col min="17" max="17" width="25.5703125" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625"/>
+    <col min="19" max="19" width="16.5703125"/>
+    <col min="20" max="20" width="19"/>
+    <col min="21" max="21" width="21.42578125" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375"/>
+    <col min="23" max="24" width="13.42578125"/>
+    <col min="25" max="25" width="19.85546875"/>
+    <col min="26" max="26" width="20.42578125" customWidth="1"/>
+    <col min="27" max="27" width="26.42578125" customWidth="1"/>
+    <col min="28" max="28" width="21"/>
+    <col min="29" max="29" width="22"/>
+    <col min="30" max="30" width="34.5703125" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" style="16"/>
+    <col min="32" max="40" width="13.42578125"/>
+    <col min="41" max="41" width="16.85546875"/>
+    <col min="42" max="42" width="19.140625"/>
+    <col min="43" max="43" width="16.28515625"/>
+    <col min="44" max="46" width="13.42578125"/>
+    <col min="47" max="47" width="19.140625"/>
+    <col min="48" max="50" width="18.140625"/>
+    <col min="51" max="51" width="0" style="2" hidden="1"/>
+    <col min="52" max="52" width="0" style="3" hidden="1"/>
+    <col min="53" max="53" width="0" style="2" hidden="1"/>
+    <col min="54" max="54" width="17.140625" style="2"/>
+    <col min="55" max="1025" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="AX1"/>
       <c r="AY1"/>
       <c r="AZ1"/>
       <c r="BA1"/>
-    </row>
-    <row r="2" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BB1"/>
+    </row>
+    <row r="2" spans="1:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3756,12 +3780,12 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AX2"/>
       <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
-    </row>
-    <row r="4" spans="1:53" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="BB2"/>
+    </row>
+    <row r="4" spans="1:54" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="6" t="s">
@@ -3795,11 +3819,12 @@
       <c r="AA4" s="30"/>
       <c r="AB4" s="30"/>
       <c r="AC4" s="30"/>
-      <c r="AD4" s="7" t="s">
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:53" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>205</v>
       </c>
@@ -3840,58 +3865,61 @@
         <v>218</v>
       </c>
       <c r="N5" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="O5" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="P5" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="R5" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="S5" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="S5" s="25" t="s">
+      <c r="T5" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="T5" s="25" t="s">
+      <c r="U5" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="V5" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="W5" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="W5" s="25" t="s">
+      <c r="X5" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="X5" s="25" t="s">
+      <c r="Y5" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="Y5" s="25" t="s">
+      <c r="Z5" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="AA5" s="25" t="s">
+      <c r="AB5" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="AB5" s="25" t="s">
+      <c r="AC5" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="AC5" s="25" t="s">
+      <c r="AD5" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="AD5" s="7" t="s">
+      <c r="AE5" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:53" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -3931,61 +3959,64 @@
       <c r="M6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="W6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="X6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Z6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AA6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AB6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AD6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AD6" s="20"/>
-      <c r="AX6"/>
+      <c r="AE6" s="20"/>
       <c r="AY6"/>
       <c r="AZ6"/>
       <c r="BA6"/>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB6"/>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
@@ -3998,8 +4029,8 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
-      <c r="N7" s="11"/>
-      <c r="P7" s="11"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -4013,10 +4044,10 @@
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
-      <c r="AD7" s="18">
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="18">
         <v>1</v>
       </c>
-      <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
@@ -4035,14 +4066,15 @@
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="11"/>
-      <c r="AX7" s="2" t="s">
+      <c r="AX7" s="11"/>
+      <c r="AY7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AZ7" s="2">
+      <c r="BA7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -4051,40 +4083,40 @@
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="AD8" s="16">
+      <c r="AE8" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D4:AC4"/>
+    <mergeCell ref="D4:AD4"/>
   </mergeCells>
   <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN7:AO7 AT7:AV7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO7:AP7 AU7:AW7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7">
       <formula1>validation_type</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7">
-      <formula1>$R$7</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
+      <formula1>$S$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH7">
       <formula1>datetype</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP7 AR7">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ7 AS7">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4092,36 +4124,36 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
       <formula1>ouinon</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:M1048576 Q7:Q1048576 B7:B1048576 T7:U1048576 G7:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:I1048576 R7:R1048576 B7:B1048576 U7:V1048576 K7:M1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="O7:O1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="P7:P1048576">
       <formula1>validation_choices</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7:V1048576">
+    <dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1048576">
       <formula1>date_choices</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AA7:AA1048576 AC7:AC1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="AB7:AB1048576 AD7:AD1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AD7:AD1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AE7:AE1048576">
       <formula1>boolean_choices</formula1>
     </dataValidation>
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="R7:S1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="S7:T1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB7:AB1048576"/>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC7:AC1048576"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -4139,13 +4171,13 @@
           <x14:formula1>
             <xm:f>metric_types!$B$3:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>Y7:Y1048576</xm:sqref>
+          <xm:sqref>Z7:Z1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>metric_units!$B$3:$B$89</xm:f>
           </x14:formula1>
-          <xm:sqref>Z7:Z1048576</xm:sqref>
+          <xm:sqref>AA7:AA1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>